<commit_message>
Fix remaining term in Jan tape; add PIF-aware validation
build_msr_tape.py:
- Add remaining_jan = remaining - 1 for all continuing Dec loans in Jan tab
- Add remaining_jan = remaining for new add loans (as-of Jan 31, already correct)
- Add rem_field parameter to write_tape_row() so Dec/Jan tabs write the right value

validate_msr_tape.py:
- Add load_pif_ids() and load_new_add_ids() to read recon files
- Auto-discover Recon_PaidInFull_*.xlsx and Recon_NewAdds_*.xlsx from script dir
- Add --pif-report and --new-add-report CLI args
- Split missing loans into PIF-explained (cleared) vs unexplained (hard stops)
- Add unconfirmed new adds as yellow lights
- Update rem term check from > to >= now that tape is correctly decremented
- Update Excel scorecard, Missing Loans sheet (two sections), and Markdown output

All output files regenerated. Hard stops: 25 → 13 (12 legit PIFs now cleared).

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Recon_Summary_Dec_2025_to_Jan_2026.xlsx
+++ b/Recon_Summary_Dec_2025_to_Jan_2026.xlsx
@@ -184,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -301,13 +301,16 @@
     <xf numFmtId="4" fontId="5" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5518,127 +5521,127 @@
     <row r="3">
       <c r="A3" s="28" t="inlineStr">
         <is>
-          <t>MSR100542</t>
+          <t>MSR100726</t>
         </is>
       </c>
       <c r="B3" s="28" t="inlineStr">
         <is>
+          <t>60 DPD</t>
+        </is>
+      </c>
+      <c r="C3" s="42" t="inlineStr">
+        <is>
           <t>Current</t>
         </is>
       </c>
-      <c r="C3" s="42" t="inlineStr">
-        <is>
-          <t>30 DPD</t>
-        </is>
-      </c>
       <c r="D3" s="13" t="n">
-        <v>251963.15</v>
+        <v>322836.07</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="36" t="inlineStr">
         <is>
-          <t>MSR100443</t>
+          <t>MSR100542</t>
         </is>
       </c>
       <c r="B4" s="36" t="inlineStr">
         <is>
-          <t>60 DPD</t>
+          <t>Current</t>
         </is>
       </c>
       <c r="C4" s="43" t="inlineStr">
         <is>
-          <t>90+ DPD</t>
+          <t>30 DPD</t>
         </is>
       </c>
       <c r="D4" s="37" t="n">
-        <v>326446.17</v>
+        <v>251963.15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="28" t="inlineStr">
         <is>
-          <t>MSR100289</t>
+          <t>MSR100195</t>
         </is>
       </c>
       <c r="B5" s="28" t="inlineStr">
         <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="C5" s="44" t="inlineStr">
+        <is>
           <t>30 DPD</t>
         </is>
       </c>
-      <c r="C5" s="44" t="inlineStr">
-        <is>
-          <t>Current</t>
-        </is>
-      </c>
       <c r="D5" s="13" t="n">
-        <v>382060.03</v>
+        <v>217167.13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="36" t="inlineStr">
         <is>
-          <t>MSR100195</t>
+          <t>MSR100869</t>
         </is>
       </c>
       <c r="B6" s="36" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>30 DPD</t>
         </is>
       </c>
       <c r="C6" s="43" t="inlineStr">
         <is>
-          <t>30 DPD</t>
+          <t>60 DPD</t>
         </is>
       </c>
       <c r="D6" s="37" t="n">
-        <v>217167.13</v>
+        <v>308607.16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="28" t="inlineStr">
         <is>
-          <t>MSR100869</t>
+          <t>MSR100499</t>
         </is>
       </c>
       <c r="B7" s="28" t="inlineStr">
         <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="C7" s="44" t="inlineStr">
+        <is>
           <t>30 DPD</t>
         </is>
       </c>
-      <c r="C7" s="42" t="inlineStr">
-        <is>
-          <t>60 DPD</t>
-        </is>
-      </c>
       <c r="D7" s="13" t="n">
-        <v>308607.16</v>
+        <v>383436.85</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="36" t="inlineStr">
         <is>
-          <t>MSR100499</t>
+          <t>MSR100289</t>
         </is>
       </c>
       <c r="B8" s="36" t="inlineStr">
         <is>
+          <t>30 DPD</t>
+        </is>
+      </c>
+      <c r="C8" s="45" t="inlineStr">
+        <is>
           <t>Current</t>
         </is>
       </c>
-      <c r="C8" s="43" t="inlineStr">
-        <is>
-          <t>30 DPD</t>
-        </is>
-      </c>
       <c r="D8" s="37" t="n">
-        <v>383436.85</v>
+        <v>382060.03</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="28" t="inlineStr">
         <is>
-          <t>MSR100726</t>
+          <t>MSR100443</t>
         </is>
       </c>
       <c r="B9" s="28" t="inlineStr">
@@ -5648,11 +5651,11 @@
       </c>
       <c r="C9" s="44" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>90+ DPD</t>
         </is>
       </c>
       <c r="D9" s="13" t="n">
-        <v>322836.07</v>
+        <v>326446.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>